<commit_message>
ID - DWR done OK - WRB done
</commit_message>
<xml_diff>
--- a/Vocabularies/OK/ok-wrb-g.xlsx
+++ b/Vocabularies/OK/ok-wrb-g.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Desktop/WSWC/IoW/Vocabularies/OK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C20ACB-0467-1D47-9E84-064A16942520}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C965925-D4B6-8942-BBCD-BDE7163E2657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="4220" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -1030,9 +1030,6 @@
     <t>Glossary: Oklahoma Water Resources Board</t>
   </si>
   <si>
-    <t>OK_WRB</t>
-  </si>
-  <si>
     <t>Oklahoma Water Resources Board</t>
   </si>
   <si>
@@ -1043,6 +1040,9 @@
   </si>
   <si>
     <t>https://www.owrb.ok.gov/util/glossary.php</t>
+  </si>
+  <si>
+    <t>OK-WRB</t>
   </si>
 </sst>
 </file>
@@ -3456,7 +3456,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3498,22 +3498,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
         <v>333</v>
       </c>
       <c r="D2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" t="s">
         <v>336</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>

</xml_diff>